<commit_message>
pattern recognition works by weakening to passage possibility for f to e.
bias is implemented by weighing distances in x different in each direction.
</commit_message>
<xml_diff>
--- a/Setup/LoadDimensions_new2021_SPT_ant.xlsx
+++ b/Setup/LoadDimensions_new2021_SPT_ant.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Name</t>
   </si>
@@ -53,16 +53,10 @@
     <t>short edge</t>
   </si>
   <si>
-    <t>9.55</t>
-  </si>
-  <si>
     <t>rounded edges</t>
   </si>
   <si>
     <t>actually measured</t>
-  </si>
-  <si>
-    <t>0.78</t>
   </si>
   <si>
     <t>9.5</t>
@@ -403,7 +397,7 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -425,7 +419,7 @@
         <v>8</v>
       </c>
       <c r="H1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -433,28 +427,28 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
         <v>14</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>13</v>
       </c>
-      <c r="D2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" t="s">
-        <v>15</v>
-      </c>
       <c r="H2" s="1">
-        <v>4.7</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>12</v>
+        <v>4.7830000000000004</v>
+      </c>
+      <c r="I2" s="1">
+        <v>9.5419999999999998</v>
+      </c>
+      <c r="J2" s="1">
+        <v>0.81</v>
       </c>
       <c r="K2" s="1">
-        <v>2.4</v>
+        <v>2.3740000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -474,19 +468,19 @@
         <v>1.17</v>
       </c>
       <c r="G3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H3" s="1">
-        <v>2.4</v>
+        <v>2.41</v>
       </c>
       <c r="I3" s="1">
-        <v>4.8</v>
+        <v>4.827</v>
       </c>
       <c r="J3" s="1">
-        <v>0.4</v>
+        <v>0.44400000000000001</v>
       </c>
       <c r="K3" s="1">
-        <v>1.2</v>
+        <v>1.2210000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -506,16 +500,16 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="H4" s="1">
-        <v>1.2</v>
+        <v>1.2250000000000001</v>
       </c>
       <c r="I4" s="1">
-        <v>2.9</v>
+        <v>2.4249999999999998</v>
       </c>
       <c r="J4" s="1">
-        <v>0.2</v>
+        <v>0.22500000000000001</v>
       </c>
       <c r="K4" s="1">
-        <v>0.6</v>
+        <v>0.622</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -535,16 +529,16 @@
         <v>0.3</v>
       </c>
       <c r="H5" s="1">
-        <v>0.6</v>
+        <v>0.627</v>
       </c>
       <c r="I5" s="1">
-        <v>1.2</v>
+        <v>1.1930000000000001</v>
       </c>
       <c r="J5" s="1">
-        <v>0.1</v>
+        <v>0.13200000000000001</v>
       </c>
       <c r="K5" s="1">
-        <v>0.3</v>
+        <v>0.32900000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>